<commit_message>
new training form & trainMemories fix + new training form changes time period every episode + fixed trainMemories: targetQ formula + added profit to be made to state + changed some hyperparameters
</commit_message>
<xml_diff>
--- a/results/simple-microsoft-5.xlsx
+++ b/results/simple-microsoft-5.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,198 @@
         <v>4.160000000000039</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-1.160000000000096</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-0.2100000000000648</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>-4.67000000000003</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>48.24999999999996</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>10.95999999999999</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-10.23999999999998</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>-12.59</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3.339999999999989</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>13.05999999999997</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>71.71999999999998</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>18.33000000000004</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-6.119999999999976</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.809999999999988</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>17.92000000000006</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>-6.989999999999981</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>-2.530000000000044</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>12.07999999999998</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>-5.519999999999982</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>64.27999999999993</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>13.09999999999989</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>-7.060000000000059</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-7.810000000000031</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>10.17000000000007</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>30.81999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>